<commit_message>
backup pc juan david
</commit_message>
<xml_diff>
--- a/Indra/volOpt/ajustes excel galileo.xlsx
+++ b/Indra/volOpt/ajustes excel galileo.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdnaranjo\Documents\documents\Indra\volOpt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20120" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -54,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -160,6 +165,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -221,7 +229,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -256,7 +264,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -471,15 +479,15 @@
       <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="59.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="59.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -493,7 +501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -508,7 +516,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -523,7 +531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -538,7 +546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -553,7 +561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -568,7 +576,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -582,14 +590,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C14" s="3"/>
     </row>
   </sheetData>
@@ -607,7 +615,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -619,7 +627,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>